<commit_message>
added confidential TSS and updated file_merger.R
</commit_message>
<xml_diff>
--- a/TSS/TSS_Master_2023.xlsx
+++ b/TSS/TSS_Master_2023.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ-CPU\Documents\GitHub\ALS-Data-Cleaning-Tool\TSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansleybr\Documents\GitHub\ALS-Data-Cleaning-Tool\TSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73561CBA-EC91-45F2-A435-3E291C9D27FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A69DD2F-CF40-4111-9B0C-E1C31D53E70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
     <sheet name="MasterData" sheetId="2" r:id="rId2"/>
-    <sheet name="probe experiment" sheetId="4" r:id="rId3"/>
-    <sheet name="Caz QAQC" sheetId="3" r:id="rId4"/>
+    <sheet name="Caz QAQC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="115">
   <si>
     <t>Column Name</t>
   </si>
@@ -287,82 +286,7 @@
     <t>DI</t>
   </si>
   <si>
-    <t>Steamboat</t>
-  </si>
-  <si>
     <t>ph, EC collected by Jake</t>
-  </si>
-  <si>
-    <t>Boulder</t>
-  </si>
-  <si>
-    <t>BOL-01-GB-4</t>
-  </si>
-  <si>
-    <t>BOL-01-GB-4-D</t>
-  </si>
-  <si>
-    <t>SCA-02-GB-4</t>
-  </si>
-  <si>
-    <t>Caz (TSS, pH, EC), Dani cleaning</t>
-  </si>
-  <si>
-    <t>SCA-02-GB-4-D</t>
-  </si>
-  <si>
-    <t>SB-02-OT-ISC-4</t>
-  </si>
-  <si>
-    <t>SB-02-OT-ISC-4-D</t>
-  </si>
-  <si>
-    <t>SCI-02-GB-4</t>
-  </si>
-  <si>
-    <t>SCI-02-GB-4-D</t>
-  </si>
-  <si>
-    <t>SCO-02-GB-4</t>
-  </si>
-  <si>
-    <t>SCO-02-GB-4-D</t>
-  </si>
-  <si>
-    <t>TR-02-GB-4</t>
-  </si>
-  <si>
-    <t>TR-02-GB-4-D</t>
-  </si>
-  <si>
-    <t>MOR-02-GB-4</t>
-  </si>
-  <si>
-    <t>MOR-02-GB-4-D</t>
-  </si>
-  <si>
-    <t>Don'y use this value in the future, bad error</t>
-  </si>
-  <si>
-    <t>Yampa</t>
-  </si>
-  <si>
-    <t>UYM-02-IN-LC-4</t>
-  </si>
-  <si>
-    <t>UYM-02-IN-LC-4-D</t>
-  </si>
-  <si>
-    <t>UYM-02-OT-ISC-4-1</t>
-  </si>
-  <si>
-    <t>UYM-02-OT-ISC-4-2</t>
-  </si>
-  <si>
-    <t>UYM-OT-ISC-4-3</t>
-  </si>
-  <si>
-    <t>UYM-OT-ISC-4-4</t>
   </si>
   <si>
     <t>Caz</t>
@@ -532,7 +456,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,12 +472,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -594,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -633,14 +551,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -938,19 +848,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="115.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="115.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -958,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -981,7 +891,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1004,7 +914,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1015,7 +925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1037,7 +947,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +958,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1059,7 +969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1070,7 +980,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1089,7 +999,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1100,7 +1010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1111,7 +1021,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1120,7 +1030,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
@@ -1128,7 +1038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1136,7 +1046,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1145,7 +1055,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1153,7 +1063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1161,7 +1071,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1169,19 +1079,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1189,7 +1099,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>53</v>
       </c>
@@ -1206,27 +1116,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B25874-14DA-4CDE-A9BC-C61EE37E0489}">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.1328125" style="12"/>
-    <col min="16" max="16" width="10.265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="12"/>
+    <col min="16" max="16" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1294,7 +1204,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>9</v>
       </c>
@@ -1302,7 +1212,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="F2" s="6">
         <v>45092</v>
@@ -1337,7 +1247,7 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T2" s="12" t="b">
         <f t="shared" ref="T2:T15" si="2">IF(G2-F2&gt;7, TRUE, FALSE)</f>
@@ -1348,10 +1258,10 @@
         <v/>
       </c>
       <c r="V2" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>9</v>
       </c>
@@ -1359,7 +1269,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="F3" s="6">
         <v>45092</v>
@@ -1394,7 +1304,7 @@
         <v>0.72299999999999998</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T3" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1405,10 +1315,10 @@
         <v/>
       </c>
       <c r="V3" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>9</v>
       </c>
@@ -1416,7 +1326,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="F4" s="6">
         <v>45092</v>
@@ -1451,7 +1361,7 @@
         <v>0.80200000000000005</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T4" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1462,10 +1372,10 @@
         <v/>
       </c>
       <c r="V4" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>9</v>
       </c>
@@ -1473,7 +1383,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F5" s="6">
         <v>45092</v>
@@ -1508,7 +1418,7 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T5" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1519,10 +1429,10 @@
         <v/>
       </c>
       <c r="V5" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>9</v>
       </c>
@@ -1530,7 +1440,7 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="F6" s="6">
         <v>45092</v>
@@ -1565,7 +1475,7 @@
         <v>0.76200000000000001</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T6" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1576,10 +1486,10 @@
         <v/>
       </c>
       <c r="V6" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>9</v>
       </c>
@@ -1587,7 +1497,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="F7" s="6">
         <v>45092</v>
@@ -1622,7 +1532,7 @@
         <v>0.748</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T7" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1633,10 +1543,10 @@
         <v/>
       </c>
       <c r="V7" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>10</v>
       </c>
@@ -1673,7 +1583,7 @@
         <v>96.666666666670821</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T8" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1684,7 +1594,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>10</v>
       </c>
@@ -1721,7 +1631,7 @@
         <v>3.3333333333329662</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T9" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1732,7 +1642,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>10</v>
       </c>
@@ -1740,7 +1650,7 @@
         <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="F10" s="6">
         <v>45092</v>
@@ -1775,7 +1685,7 @@
         <v>0.75600000000000001</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T10" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1786,10 +1696,10 @@
         <v/>
       </c>
       <c r="V10" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -1797,7 +1707,7 @@
         <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F11" s="6">
         <v>45092</v>
@@ -1832,7 +1742,7 @@
         <v>0.753</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T11" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1843,10 +1753,10 @@
         <v/>
       </c>
       <c r="V11" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -1854,7 +1764,7 @@
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="F12" s="6">
         <v>45092</v>
@@ -1889,7 +1799,7 @@
         <v>0.82499999999999996</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T12" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1900,10 +1810,10 @@
         <v/>
       </c>
       <c r="V12" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1911,7 +1821,7 @@
         <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F13" s="6">
         <v>45092</v>
@@ -1946,7 +1856,7 @@
         <v>0.82</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T13" s="12" t="b">
         <f t="shared" si="2"/>
@@ -1957,10 +1867,10 @@
         <v/>
       </c>
       <c r="V13" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>10</v>
       </c>
@@ -1968,7 +1878,7 @@
         <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="F14" s="6">
         <v>45092</v>
@@ -2003,7 +1913,7 @@
         <v>0.97399999999999998</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T14" s="12" t="b">
         <f t="shared" si="2"/>
@@ -2014,10 +1924,10 @@
         <v/>
       </c>
       <c r="V14" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>10</v>
       </c>
@@ -2025,7 +1935,7 @@
         <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="F15" s="6">
         <v>45092</v>
@@ -2060,7 +1970,7 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="S15" s="12" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="T15" s="12" t="b">
         <f t="shared" si="2"/>
@@ -2071,10 +1981,10 @@
         <v/>
       </c>
       <c r="V15" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>15</v>
       </c>
@@ -2117,7 +2027,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
@@ -2160,7 +2070,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
@@ -2168,7 +2078,7 @@
         <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="F18" s="6">
         <v>45124</v>
@@ -2203,7 +2113,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>15</v>
       </c>
@@ -2211,7 +2121,7 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="F19" s="6">
         <v>45124</v>
@@ -2246,7 +2156,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>15</v>
       </c>
@@ -2254,7 +2164,7 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="F20" s="6">
         <v>45124</v>
@@ -2287,7 +2197,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>15</v>
       </c>
@@ -2295,7 +2205,7 @@
         <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="F21" s="6">
         <v>45124</v>
@@ -2328,7 +2238,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>15</v>
       </c>
@@ -2336,7 +2246,7 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="F22" s="6">
         <v>45124</v>
@@ -2369,7 +2279,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>15</v>
       </c>
@@ -2377,7 +2287,7 @@
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="F23" s="6">
         <v>45124</v>
@@ -2410,7 +2320,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>15</v>
       </c>
@@ -2418,7 +2328,7 @@
         <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="F24" s="6">
         <v>45124</v>
@@ -2451,7 +2361,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>15</v>
       </c>
@@ -2459,7 +2369,7 @@
         <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F25" s="6">
         <v>45124</v>
@@ -2492,7 +2402,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>15</v>
       </c>
@@ -2500,7 +2410,7 @@
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="F26" s="6">
         <v>45124</v>
@@ -2533,7 +2443,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>15</v>
       </c>
@@ -2541,7 +2451,7 @@
         <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="F27" s="6">
         <v>45124</v>
@@ -2574,7 +2484,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>16</v>
       </c>
@@ -2615,7 +2525,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>16</v>
       </c>
@@ -2656,7 +2566,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>16</v>
       </c>
@@ -2664,7 +2574,7 @@
         <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="F30" s="6">
         <v>45124</v>
@@ -2697,7 +2607,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>16</v>
       </c>
@@ -2705,7 +2615,7 @@
         <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="F31" s="6">
         <v>45124</v>
@@ -2738,7 +2648,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>16</v>
       </c>
@@ -2746,7 +2656,7 @@
         <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="F32" s="6">
         <v>45124</v>
@@ -2779,7 +2689,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>16</v>
       </c>
@@ -2787,7 +2697,7 @@
         <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="F33" s="6">
         <v>45124</v>
@@ -2820,7 +2730,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>16</v>
       </c>
@@ -2828,7 +2738,7 @@
         <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="F34" s="6">
         <v>45124</v>
@@ -2861,7 +2771,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>16</v>
       </c>
@@ -2869,7 +2779,7 @@
         <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F35" s="6">
         <v>45124</v>
@@ -2902,7 +2812,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>16</v>
       </c>
@@ -2910,7 +2820,7 @@
         <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="F36" s="6">
         <v>45124</v>
@@ -2943,7 +2853,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>16</v>
       </c>
@@ -2951,7 +2861,7 @@
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="F37" s="6">
         <v>45124</v>
@@ -2984,7 +2894,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>16</v>
       </c>
@@ -2992,7 +2902,7 @@
         <v>62</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F38" s="6">
         <v>45124</v>
@@ -3025,7 +2935,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>16</v>
       </c>
@@ -3033,7 +2943,7 @@
         <v>63</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="F39" s="6">
         <v>45124</v>
@@ -3066,7 +2976,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>17</v>
       </c>
@@ -3103,7 +3013,7 @@
         <v>103.33333333332936</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>17</v>
       </c>
@@ -3140,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>17</v>
       </c>
@@ -3148,7 +3058,7 @@
         <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="F42" s="6">
         <v>45124</v>
@@ -3177,7 +3087,7 @@
         <v>383.33333333332814</v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>17</v>
       </c>
@@ -3185,7 +3095,7 @@
         <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="F43" s="6">
         <v>45124</v>
@@ -3214,7 +3124,7 @@
         <v>1563.3333333333314</v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>17</v>
       </c>
@@ -3222,7 +3132,7 @@
         <v>34</v>
       </c>
       <c r="D44" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="F44" s="6">
         <v>45124</v>
@@ -3251,7 +3161,7 @@
         <v>1886.6666666666661</v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>17</v>
       </c>
@@ -3259,7 +3169,7 @@
         <v>35</v>
       </c>
       <c r="D45" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="F45" s="6">
         <v>45124</v>
@@ -3288,7 +3198,7 @@
         <v>1450.0000000000032</v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="I46" s="12"/>
@@ -3302,2214 +3212,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72DA8E6-28C6-4FBA-8CF2-04F8551A4743}">
-  <dimension ref="A1:V42"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="4" max="4" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.73046875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="12">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>45058</v>
-      </c>
-      <c r="G2" s="6">
-        <v>45067</v>
-      </c>
-      <c r="H2" s="6">
-        <v>45068</v>
-      </c>
-      <c r="I2" s="12">
-        <v>30</v>
-      </c>
-      <c r="J2">
-        <v>1.1921999999999999</v>
-      </c>
-      <c r="K2">
-        <v>1.1929000000000001</v>
-      </c>
-      <c r="M2" s="14">
-        <f>(SMALL(K2:L2,1)-J2)*1000</f>
-        <v>0.70000000000014495</v>
-      </c>
-      <c r="N2" s="14">
-        <f>M2/(I2/1000)</f>
-        <v>23.333333333338167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="12">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>119</v>
-      </c>
-      <c r="D3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
-        <v>45058</v>
-      </c>
-      <c r="G3" s="6">
-        <v>45070</v>
-      </c>
-      <c r="H3" s="6">
-        <v>45071</v>
-      </c>
-      <c r="I3" s="12">
-        <v>30</v>
-      </c>
-      <c r="J3">
-        <v>1.1861999999999999</v>
-      </c>
-      <c r="K3">
-        <v>1.1867000000000001</v>
-      </c>
-      <c r="M3" s="14">
-        <f t="shared" ref="M3" si="0">(SMALL(K3:L3,1)-J3)*1000</f>
-        <v>0.50000000000016698</v>
-      </c>
-      <c r="N3" s="14">
-        <f t="shared" ref="N3" si="1">M3/(I3/1000)</f>
-        <v>16.666666666672235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="12">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>45058</v>
-      </c>
-      <c r="G4" s="6">
-        <v>45067</v>
-      </c>
-      <c r="H4" s="6">
-        <v>45068</v>
-      </c>
-      <c r="I4" s="12">
-        <v>30</v>
-      </c>
-      <c r="J4">
-        <v>1.2146999999999999</v>
-      </c>
-      <c r="K4">
-        <v>1.2158</v>
-      </c>
-      <c r="M4" s="14">
-        <f>(SMALL(K4:L4,1)-J4)*1000</f>
-        <v>1.1000000000001009</v>
-      </c>
-      <c r="N4" s="14">
-        <f>M4/(I4/1000)</f>
-        <v>36.666666666670032</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="12">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>45058</v>
-      </c>
-      <c r="G5" s="6">
-        <v>45070</v>
-      </c>
-      <c r="H5" s="6">
-        <v>45071</v>
-      </c>
-      <c r="I5" s="12">
-        <v>30</v>
-      </c>
-      <c r="J5">
-        <v>1.2131000000000001</v>
-      </c>
-      <c r="K5">
-        <v>1.2137</v>
-      </c>
-      <c r="M5" s="14">
-        <f t="shared" ref="M5:M9" si="2">(SMALL(K5:L5,1)-J5)*1000</f>
-        <v>0.59999999999993392</v>
-      </c>
-      <c r="N5" s="14">
-        <f t="shared" ref="N5:N9" si="3">M5/(I5/1000)</f>
-        <v>19.999999999997797</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="12">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>120</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>45058</v>
-      </c>
-      <c r="G6" s="6">
-        <v>45070</v>
-      </c>
-      <c r="H6" s="6">
-        <v>45071</v>
-      </c>
-      <c r="I6" s="12">
-        <v>30</v>
-      </c>
-      <c r="J6">
-        <v>1.2131000000000001</v>
-      </c>
-      <c r="K6">
-        <v>1.2138</v>
-      </c>
-      <c r="M6" s="14">
-        <f t="shared" si="2"/>
-        <v>0.69999999999992291</v>
-      </c>
-      <c r="N6" s="14">
-        <f t="shared" si="3"/>
-        <v>23.333333333330764</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="12">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G7" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H7" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I7" s="12">
-        <v>30</v>
-      </c>
-      <c r="J7">
-        <v>1.2096</v>
-      </c>
-      <c r="K7">
-        <v>1.2105999999999999</v>
-      </c>
-      <c r="M7" s="14">
-        <f t="shared" si="2"/>
-        <v>0.99999999999988987</v>
-      </c>
-      <c r="N7" s="14">
-        <f t="shared" si="3"/>
-        <v>33.333333333329662</v>
-      </c>
-      <c r="O7" s="12">
-        <v>8.18</v>
-      </c>
-      <c r="P7" s="12">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>45082.486111111109</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T7" s="12" t="b">
-        <f t="shared" ref="T7" si="4">IF(G7-F7&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="12" t="str">
-        <f t="shared" ref="U7" si="5">IF(AND(D7="Stock Solution", N7&gt;=90, N7&lt;=110), "Good", IF(AND(D7="DI", N7&gt;=-3.33, N7&lt;=3.33), "Good", IF(OR(D7&lt;&gt;"Stock Solution", D7&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G8" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H8" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I8" s="12">
-        <v>30</v>
-      </c>
-      <c r="J8">
-        <v>1.2172000000000001</v>
-      </c>
-      <c r="K8">
-        <v>1.2182999999999999</v>
-      </c>
-      <c r="M8" s="18">
-        <f t="shared" si="2"/>
-        <v>1.0999999999998789</v>
-      </c>
-      <c r="N8" s="18">
-        <f t="shared" si="3"/>
-        <v>36.666666666662628</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="12">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G9" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H9" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I9" s="12">
-        <v>30</v>
-      </c>
-      <c r="J9">
-        <v>1.2133</v>
-      </c>
-      <c r="K9">
-        <v>1.2145999999999999</v>
-      </c>
-      <c r="M9" s="14">
-        <f t="shared" si="2"/>
-        <v>1.2999999999998568</v>
-      </c>
-      <c r="N9" s="14">
-        <f t="shared" si="3"/>
-        <v>43.333333333328561</v>
-      </c>
-      <c r="O9" s="12">
-        <v>8.15</v>
-      </c>
-      <c r="P9" s="12">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="Q9" s="16">
-        <v>45082.486111111109</v>
-      </c>
-      <c r="S9" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T9" s="12" t="b">
-        <f t="shared" ref="T9" si="6">IF(G9-F9&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U9" s="12" t="str">
-        <f t="shared" ref="U9" si="7">IF(AND(D9="Stock Solution", N9&gt;=90, N9&lt;=110), "Good", IF(AND(D9="DI", N9&gt;=-3.33, N9&lt;=3.33), "Good", IF(OR(D9&lt;&gt;"Stock Solution", D9&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G10" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H10" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I10" s="12">
-        <v>30</v>
-      </c>
-      <c r="J10">
-        <v>1.2161999999999999</v>
-      </c>
-      <c r="K10">
-        <v>1.2173</v>
-      </c>
-      <c r="M10" s="18">
-        <f t="shared" ref="M10:M11" si="8">(SMALL(K10:L10,1)-J10)*1000</f>
-        <v>1.1000000000001009</v>
-      </c>
-      <c r="N10" s="18">
-        <f t="shared" ref="N10:N11" si="9">M10/(I10/1000)</f>
-        <v>36.666666666670032</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="12">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G11" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H11" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I11" s="12">
-        <v>30</v>
-      </c>
-      <c r="J11">
-        <v>1.2211000000000001</v>
-      </c>
-      <c r="K11">
-        <v>1.2218</v>
-      </c>
-      <c r="M11" s="14">
-        <f t="shared" si="8"/>
-        <v>0.69999999999992291</v>
-      </c>
-      <c r="N11" s="14">
-        <f t="shared" si="9"/>
-        <v>23.333333333330764</v>
-      </c>
-      <c r="O11" s="12">
-        <v>8.25</v>
-      </c>
-      <c r="P11" s="12">
-        <v>0.33100000000000002</v>
-      </c>
-      <c r="Q11" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S11" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T11" s="12" t="b">
-        <f t="shared" ref="T11" si="10">IF(G11-F11&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U11" s="12" t="str">
-        <f t="shared" ref="U11" si="11">IF(AND(D11="Stock Solution", N11&gt;=90, N11&lt;=110), "Good", IF(AND(D11="DI", N11&gt;=-3.33, N11&lt;=3.33), "Good", IF(OR(D11&lt;&gt;"Stock Solution", D11&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G12" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H12" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I12" s="12">
-        <v>30</v>
-      </c>
-      <c r="J12">
-        <v>1.2281</v>
-      </c>
-      <c r="K12">
-        <v>1.2290000000000001</v>
-      </c>
-      <c r="M12" s="18">
-        <f t="shared" ref="M12:M13" si="12">(SMALL(K12:L12,1)-J12)*1000</f>
-        <v>0.90000000000012292</v>
-      </c>
-      <c r="N12" s="18">
-        <f t="shared" ref="N12:N13" si="13">M12/(I12/1000)</f>
-        <v>30.0000000000041</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="12">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G13" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H13" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I13" s="12">
-        <v>30</v>
-      </c>
-      <c r="J13">
-        <v>1.2148000000000001</v>
-      </c>
-      <c r="K13">
-        <v>1.2156</v>
-      </c>
-      <c r="M13" s="14">
-        <f t="shared" si="12"/>
-        <v>0.79999999999991189</v>
-      </c>
-      <c r="N13" s="14">
-        <f t="shared" si="13"/>
-        <v>26.66666666666373</v>
-      </c>
-      <c r="O13" s="12">
-        <v>8.24</v>
-      </c>
-      <c r="P13" s="12">
-        <v>0.33200000000000002</v>
-      </c>
-      <c r="Q13" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T13" s="12" t="b">
-        <f t="shared" ref="T13" si="14">IF(G13-F13&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U13" s="12" t="str">
-        <f t="shared" ref="U13" si="15">IF(AND(D13="Stock Solution", N13&gt;=90, N13&lt;=110), "Good", IF(AND(D13="DI", N13&gt;=-3.33, N13&lt;=3.33), "Good", IF(OR(D13&lt;&gt;"Stock Solution", D13&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G14" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H14" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I14" s="12">
-        <v>30</v>
-      </c>
-      <c r="J14">
-        <v>1.2161999999999999</v>
-      </c>
-      <c r="K14">
-        <v>1.2171000000000001</v>
-      </c>
-      <c r="M14" s="18">
-        <f t="shared" ref="M14:M15" si="16">(SMALL(K14:L14,1)-J14)*1000</f>
-        <v>0.90000000000012292</v>
-      </c>
-      <c r="N14" s="18">
-        <f t="shared" ref="N14:N15" si="17">M14/(I14/1000)</f>
-        <v>30.0000000000041</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="12">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G15" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H15" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I15" s="12">
-        <v>30</v>
-      </c>
-      <c r="J15">
-        <v>1.2181999999999999</v>
-      </c>
-      <c r="K15">
-        <v>1.2184999999999999</v>
-      </c>
-      <c r="M15" s="14">
-        <f t="shared" si="16"/>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N15" s="14">
-        <f t="shared" si="17"/>
-        <v>9.9999999999988987</v>
-      </c>
-      <c r="O15" s="12">
-        <v>8.36</v>
-      </c>
-      <c r="P15" s="12">
-        <v>0.38800000000000001</v>
-      </c>
-      <c r="Q15" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S15" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T15" s="12" t="b">
-        <f t="shared" ref="T15" si="18">IF(G15-F15&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U15" s="12" t="str">
-        <f t="shared" ref="U15" si="19">IF(AND(D15="Stock Solution", N15&gt;=90, N15&lt;=110), "Good", IF(AND(D15="DI", N15&gt;=-3.33, N15&lt;=3.33), "Good", IF(OR(D15&lt;&gt;"Stock Solution", D15&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G16" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H16" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I16" s="12">
-        <v>30</v>
-      </c>
-      <c r="J16">
-        <v>1.1956</v>
-      </c>
-      <c r="K16">
-        <v>1.1959</v>
-      </c>
-      <c r="M16" s="18">
-        <f t="shared" ref="M16:M17" si="20">(SMALL(K16:L16,1)-J16)*1000</f>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N16" s="18">
-        <f t="shared" ref="N16:N17" si="21">M16/(I16/1000)</f>
-        <v>9.9999999999988987</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="12">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G17" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H17" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I17" s="12">
-        <v>30</v>
-      </c>
-      <c r="J17">
-        <v>1.2131000000000001</v>
-      </c>
-      <c r="K17">
-        <v>1.2134</v>
-      </c>
-      <c r="M17" s="14">
-        <f t="shared" si="20"/>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N17" s="14">
-        <f t="shared" si="21"/>
-        <v>9.9999999999988987</v>
-      </c>
-      <c r="O17" s="12">
-        <v>8.3699999999999992</v>
-      </c>
-      <c r="P17" s="12">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="Q17" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S17" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T17" s="12" t="b">
-        <f t="shared" ref="T17" si="22">IF(G17-F17&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U17" s="12" t="str">
-        <f t="shared" ref="U17" si="23">IF(AND(D17="Stock Solution", N17&gt;=90, N17&lt;=110), "Good", IF(AND(D17="DI", N17&gt;=-3.33, N17&lt;=3.33), "Good", IF(OR(D17&lt;&gt;"Stock Solution", D17&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G18" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H18" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I18" s="12">
-        <v>30</v>
-      </c>
-      <c r="J18">
-        <v>1.1971000000000001</v>
-      </c>
-      <c r="K18">
-        <v>1.1978</v>
-      </c>
-      <c r="M18" s="18">
-        <f t="shared" ref="M18:M19" si="24">(SMALL(K18:L18,1)-J18)*1000</f>
-        <v>0.69999999999992291</v>
-      </c>
-      <c r="N18" s="18">
-        <f t="shared" ref="N18:N19" si="25">M18/(I18/1000)</f>
-        <v>23.333333333330764</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="12">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G19" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H19" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I19" s="12">
-        <v>30</v>
-      </c>
-      <c r="J19">
-        <v>1.2038</v>
-      </c>
-      <c r="K19">
-        <v>1.2039</v>
-      </c>
-      <c r="M19" s="14">
-        <f t="shared" si="24"/>
-        <v>9.9999999999988987E-2</v>
-      </c>
-      <c r="N19" s="14">
-        <f t="shared" si="25"/>
-        <v>3.3333333333329662</v>
-      </c>
-      <c r="O19" s="12">
-        <v>8.4700000000000006</v>
-      </c>
-      <c r="P19" s="12">
-        <v>0.39</v>
-      </c>
-      <c r="Q19" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S19" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T19" s="12" t="b">
-        <f t="shared" ref="T19" si="26">IF(G19-F19&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U19" s="12" t="str">
-        <f t="shared" ref="U19" si="27">IF(AND(D19="Stock Solution", N19&gt;=90, N19&lt;=110), "Good", IF(AND(D19="DI", N19&gt;=-3.33, N19&lt;=3.33), "Good", IF(OR(D19&lt;&gt;"Stock Solution", D19&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>40</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G20" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H20" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I20" s="12">
-        <v>30</v>
-      </c>
-      <c r="J20">
-        <v>1.2015</v>
-      </c>
-      <c r="K20">
-        <v>1.2016</v>
-      </c>
-      <c r="M20" s="18">
-        <f t="shared" ref="M20:M21" si="28">(SMALL(K20:L20,1)-J20)*1000</f>
-        <v>9.9999999999988987E-2</v>
-      </c>
-      <c r="N20" s="18">
-        <f t="shared" ref="N20:N21" si="29">M20/(I20/1000)</f>
-        <v>3.3333333333329662</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="12">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G21" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H21" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I21" s="12">
-        <v>30</v>
-      </c>
-      <c r="J21">
-        <v>1.2197</v>
-      </c>
-      <c r="K21">
-        <v>1.22</v>
-      </c>
-      <c r="M21" s="14">
-        <f t="shared" si="28"/>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N21" s="14">
-        <f t="shared" si="29"/>
-        <v>9.9999999999988987</v>
-      </c>
-      <c r="O21" s="12">
-        <v>8.42</v>
-      </c>
-      <c r="P21" s="12">
-        <v>0.39</v>
-      </c>
-      <c r="Q21" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S21" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T21" s="12" t="b">
-        <f t="shared" ref="T21" si="30">IF(G21-F21&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U21" s="12" t="str">
-        <f t="shared" ref="U21" si="31">IF(AND(D21="Stock Solution", N21&gt;=90, N21&lt;=110), "Good", IF(AND(D21="DI", N21&gt;=-3.33, N21&lt;=3.33), "Good", IF(OR(D21&lt;&gt;"Stock Solution", D21&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G22" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H22" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I22" s="12">
-        <v>30</v>
-      </c>
-      <c r="J22">
-        <v>1.2314000000000001</v>
-      </c>
-      <c r="K22">
-        <v>1.2317</v>
-      </c>
-      <c r="M22" s="18">
-        <f t="shared" ref="M22:M27" si="32">(SMALL(K22:L22,1)-J22)*1000</f>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N22" s="18">
-        <f t="shared" ref="N22:N27" si="33">M22/(I22/1000)</f>
-        <v>9.9999999999988987</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="12">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G23" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H23" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I23" s="12">
-        <v>30</v>
-      </c>
-      <c r="J23">
-        <v>1.1967000000000001</v>
-      </c>
-      <c r="K23">
-        <v>1.1975</v>
-      </c>
-      <c r="M23" s="14">
-        <f t="shared" si="32"/>
-        <v>0.79999999999991189</v>
-      </c>
-      <c r="N23" s="14">
-        <f t="shared" si="33"/>
-        <v>26.66666666666373</v>
-      </c>
-      <c r="O23" s="12">
-        <v>8.2200000000000006</v>
-      </c>
-      <c r="P23" s="12">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="Q23" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S23" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T23" s="12" t="b">
-        <f t="shared" ref="T23" si="34">IF(G23-F23&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U23" s="12" t="str">
-        <f t="shared" ref="U23" si="35">IF(AND(D23="Stock Solution", N23&gt;=90, N23&lt;=110), "Good", IF(AND(D23="DI", N23&gt;=-3.33, N23&lt;=3.33), "Good", IF(OR(D23&lt;&gt;"Stock Solution", D23&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24">
-        <v>49</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G24" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H24" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I24" s="12">
-        <v>30</v>
-      </c>
-      <c r="J24">
-        <v>1.2144999999999999</v>
-      </c>
-      <c r="K24">
-        <v>1.2149000000000001</v>
-      </c>
-      <c r="M24" s="18">
-        <f t="shared" si="32"/>
-        <v>0.40000000000017799</v>
-      </c>
-      <c r="N24" s="18">
-        <f t="shared" si="33"/>
-        <v>13.333333333339267</v>
-      </c>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="12">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G25" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H25" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I25" s="12">
-        <v>30</v>
-      </c>
-      <c r="J25">
-        <v>1.2123999999999999</v>
-      </c>
-      <c r="K25">
-        <v>1.2132000000000001</v>
-      </c>
-      <c r="M25" s="14">
-        <f t="shared" si="32"/>
-        <v>0.80000000000013394</v>
-      </c>
-      <c r="N25" s="14">
-        <f t="shared" si="33"/>
-        <v>26.666666666671134</v>
-      </c>
-      <c r="O25" s="12">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="P25" s="12">
-        <v>0.154</v>
-      </c>
-      <c r="Q25" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S25" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T25" s="12" t="b">
-        <f t="shared" ref="T25" si="36">IF(G25-F25&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U25" s="12" t="str">
-        <f t="shared" ref="U25" si="37">IF(AND(D25="Stock Solution", N25&gt;=90, N25&lt;=110), "Good", IF(AND(D25="DI", N25&gt;=-3.33, N25&lt;=3.33), "Good", IF(OR(D25&lt;&gt;"Stock Solution", D25&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26">
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
-      <c r="F26" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G26" s="6">
-        <v>45097</v>
-      </c>
-      <c r="H26" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I26" s="12">
-        <v>30</v>
-      </c>
-      <c r="J26">
-        <v>1.1976</v>
-      </c>
-      <c r="K26">
-        <v>1.1984999999999999</v>
-      </c>
-      <c r="M26" s="18">
-        <f t="shared" si="32"/>
-        <v>0.89999999999990088</v>
-      </c>
-      <c r="N26" s="18">
-        <f t="shared" si="33"/>
-        <v>29.999999999996696</v>
-      </c>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="12">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G27" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H27" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I27" s="12">
-        <v>30</v>
-      </c>
-      <c r="J27">
-        <v>1.2065999999999999</v>
-      </c>
-      <c r="K27">
-        <v>1.2074</v>
-      </c>
-      <c r="M27" s="14">
-        <f t="shared" si="32"/>
-        <v>0.80000000000013394</v>
-      </c>
-      <c r="N27" s="14">
-        <f t="shared" si="33"/>
-        <v>26.666666666671134</v>
-      </c>
-      <c r="O27" s="12">
-        <v>7.72</v>
-      </c>
-      <c r="P27" s="12">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="Q27" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S27" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T27" s="12" t="b">
-        <f t="shared" ref="T27" si="38">IF(G27-F27&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U27" s="12" t="str">
-        <f t="shared" ref="U27" si="39">IF(AND(D27="Stock Solution", N27&gt;=90, N27&lt;=110), "Good", IF(AND(D27="DI", N27&gt;=-3.33, N27&lt;=3.33), "Good", IF(OR(D27&lt;&gt;"Stock Solution", D27&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28">
-        <v>8</v>
-      </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="F28" s="6">
-        <v>45097</v>
-      </c>
-      <c r="G28" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H28" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I28" s="12">
-        <v>30</v>
-      </c>
-      <c r="J28">
-        <v>1.2141</v>
-      </c>
-      <c r="K28">
-        <v>1.2151000000000001</v>
-      </c>
-      <c r="M28" s="18">
-        <f t="shared" ref="M28:M42" si="40">(SMALL(K28:L28,1)-J28)*1000</f>
-        <v>1.0000000000001119</v>
-      </c>
-      <c r="N28" s="18">
-        <f t="shared" ref="N28:N42" si="41">M28/(I28/1000)</f>
-        <v>33.333333333337066</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="B29" s="12">
-        <v>5</v>
-      </c>
-      <c r="C29">
-        <v>48</v>
-      </c>
-      <c r="D29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" t="b">
-        <v>0</v>
-      </c>
-      <c r="F29" s="6">
-        <v>45078</v>
-      </c>
-      <c r="G29" s="6">
-        <v>45081</v>
-      </c>
-      <c r="H29" s="6">
-        <v>45085</v>
-      </c>
-      <c r="I29" s="12">
-        <v>30</v>
-      </c>
-      <c r="J29">
-        <v>1.2017</v>
-      </c>
-      <c r="K29">
-        <v>1.2114</v>
-      </c>
-      <c r="M29" s="18">
-        <f t="shared" si="40"/>
-        <v>9.7000000000000419</v>
-      </c>
-      <c r="N29" s="18">
-        <f t="shared" si="41"/>
-        <v>323.33333333333474</v>
-      </c>
-      <c r="O29" s="12">
-        <v>7.51</v>
-      </c>
-      <c r="P29" s="12">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="Q29" s="16">
-        <v>45082.486111053244</v>
-      </c>
-      <c r="S29" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T29" s="12" t="b">
-        <f t="shared" ref="T29" si="42">IF(G29-F29&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U29" s="12" t="str">
-        <f t="shared" ref="U29" si="43">IF(AND(D29="Stock Solution", N29&gt;=90, N29&lt;=110), "Good", IF(AND(D29="DI", N29&gt;=-3.33, N29&lt;=3.33), "Good", IF(OR(D29&lt;&gt;"Stock Solution", D29&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-      <c r="V29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A30" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" s="20">
-        <v>8</v>
-      </c>
-      <c r="C30" s="20">
-        <v>5</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="21">
-        <v>45078</v>
-      </c>
-      <c r="G30" s="21">
-        <v>45098</v>
-      </c>
-      <c r="H30" s="21">
-        <v>45102</v>
-      </c>
-      <c r="I30" s="22">
-        <v>30</v>
-      </c>
-      <c r="J30" s="20">
-        <v>1.2144999999999999</v>
-      </c>
-      <c r="K30" s="20">
-        <v>1.2154</v>
-      </c>
-      <c r="L30" s="20"/>
-      <c r="M30" s="23">
-        <f t="shared" si="40"/>
-        <v>0.90000000000012292</v>
-      </c>
-      <c r="N30" s="23">
-        <f t="shared" si="41"/>
-        <v>30.0000000000041</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="12">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>25</v>
-      </c>
-      <c r="D31" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F31" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G31" s="6">
-        <v>45089</v>
-      </c>
-      <c r="H31" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I31" s="12">
-        <v>30</v>
-      </c>
-      <c r="J31">
-        <v>1.2020999999999999</v>
-      </c>
-      <c r="K31">
-        <v>1.2020999999999999</v>
-      </c>
-      <c r="M31" s="18">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="18">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="12">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="P31" s="12">
-        <v>0.16</v>
-      </c>
-      <c r="Q31" s="16">
-        <v>45091.125</v>
-      </c>
-      <c r="S31" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T31" s="12" t="b">
-        <f t="shared" ref="T31" si="44">IF(G31-F31&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U31" s="12" t="str">
-        <f t="shared" ref="U31" si="45">IF(AND(D31="Stock Solution", N31&gt;=90, N31&lt;=110), "Good", IF(AND(D31="DI", N31&gt;=-3.33, N31&lt;=3.33), "Good", IF(OR(D31&lt;&gt;"Stock Solution", D31&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32">
-        <v>8</v>
-      </c>
-      <c r="C32">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G32" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H32" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I32" s="12">
-        <v>30</v>
-      </c>
-      <c r="J32">
-        <v>1.2205999999999999</v>
-      </c>
-      <c r="K32">
-        <v>1.2212000000000001</v>
-      </c>
-      <c r="M32" s="18">
-        <f t="shared" si="40"/>
-        <v>0.60000000000015596</v>
-      </c>
-      <c r="N32" s="18">
-        <f t="shared" si="41"/>
-        <v>20.000000000005201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="12">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>26</v>
-      </c>
-      <c r="D33" t="s">
-        <v>97</v>
-      </c>
-      <c r="E33" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G33" s="6">
-        <v>45089</v>
-      </c>
-      <c r="H33" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I33" s="12">
-        <v>30</v>
-      </c>
-      <c r="J33">
-        <v>1.1915</v>
-      </c>
-      <c r="K33">
-        <v>1.1915</v>
-      </c>
-      <c r="M33" s="18">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="18">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="O33" s="12">
-        <v>7.99</v>
-      </c>
-      <c r="P33" s="12">
-        <v>0.16</v>
-      </c>
-      <c r="Q33" s="16">
-        <v>45091.125</v>
-      </c>
-      <c r="S33" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T33" s="12" t="b">
-        <f t="shared" ref="T33" si="46">IF(G33-F33&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U33" s="12" t="str">
-        <f t="shared" ref="U33" si="47">IF(AND(D33="Stock Solution", N33&gt;=90, N33&lt;=110), "Good", IF(AND(D33="DI", N33&gt;=-3.33, N33&lt;=3.33), "Good", IF(OR(D33&lt;&gt;"Stock Solution", D33&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G34" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H34" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I34" s="12">
-        <v>30</v>
-      </c>
-      <c r="J34">
-        <v>1.2158</v>
-      </c>
-      <c r="K34">
-        <v>1.2166999999999999</v>
-      </c>
-      <c r="M34" s="18">
-        <f t="shared" si="40"/>
-        <v>0.89999999999990088</v>
-      </c>
-      <c r="N34" s="18">
-        <f t="shared" si="41"/>
-        <v>29.999999999996696</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B35" s="12">
-        <v>6</v>
-      </c>
-      <c r="C35">
-        <v>27</v>
-      </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G35" s="6">
-        <v>45089</v>
-      </c>
-      <c r="H35" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I35" s="12">
-        <v>30</v>
-      </c>
-      <c r="J35">
-        <v>1.214</v>
-      </c>
-      <c r="K35">
-        <v>1.2142999999999999</v>
-      </c>
-      <c r="M35" s="18">
-        <f t="shared" si="40"/>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N35" s="18">
-        <f t="shared" si="41"/>
-        <v>9.9999999999988987</v>
-      </c>
-      <c r="O35" s="12">
-        <v>7.89</v>
-      </c>
-      <c r="P35" s="12">
-        <v>0.21</v>
-      </c>
-      <c r="Q35" s="16">
-        <v>45091.125</v>
-      </c>
-      <c r="S35" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T35" s="12" t="b">
-        <f t="shared" ref="T35" si="48">IF(G35-F35&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U35" s="12" t="str">
-        <f t="shared" ref="U35" si="49">IF(AND(D35="Stock Solution", N35&gt;=90, N35&lt;=110), "Good", IF(AND(D35="DI", N35&gt;=-3.33, N35&lt;=3.33), "Good", IF(OR(D35&lt;&gt;"Stock Solution", D35&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36">
-        <v>8</v>
-      </c>
-      <c r="C36">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>98</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G36" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H36" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I36" s="12">
-        <v>30</v>
-      </c>
-      <c r="J36">
-        <v>1.2175</v>
-      </c>
-      <c r="K36">
-        <v>1.2181</v>
-      </c>
-      <c r="M36" s="18">
-        <f t="shared" si="40"/>
-        <v>0.59999999999993392</v>
-      </c>
-      <c r="N36" s="18">
-        <f t="shared" si="41"/>
-        <v>19.999999999997797</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37">
-        <v>28</v>
-      </c>
-      <c r="D37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G37" s="6">
-        <v>45089</v>
-      </c>
-      <c r="H37" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I37" s="12">
-        <v>30</v>
-      </c>
-      <c r="J37">
-        <v>1.1974</v>
-      </c>
-      <c r="K37">
-        <v>1.1976</v>
-      </c>
-      <c r="M37" s="18">
-        <f t="shared" si="40"/>
-        <v>0.19999999999997797</v>
-      </c>
-      <c r="N37" s="18">
-        <f t="shared" si="41"/>
-        <v>6.6666666666659324</v>
-      </c>
-      <c r="O37" s="12">
-        <v>8.02</v>
-      </c>
-      <c r="P37" s="12">
-        <v>0.23</v>
-      </c>
-      <c r="Q37" s="16">
-        <v>45091.125</v>
-      </c>
-      <c r="S37" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T37" s="12" t="b">
-        <f t="shared" ref="T37" si="50">IF(G37-F37&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U37" s="12" t="str">
-        <f t="shared" ref="U37" si="51">IF(AND(D37="Stock Solution", N37&gt;=90, N37&lt;=110), "Good", IF(AND(D37="DI", N37&gt;=-3.33, N37&lt;=3.33), "Good", IF(OR(D37&lt;&gt;"Stock Solution", D37&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38">
-        <v>8</v>
-      </c>
-      <c r="C38">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G38" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H38" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I38" s="12">
-        <v>30</v>
-      </c>
-      <c r="J38">
-        <v>1.2168000000000001</v>
-      </c>
-      <c r="K38">
-        <v>1.2173</v>
-      </c>
-      <c r="M38" s="18">
-        <f t="shared" si="40"/>
-        <v>0.49999999999994493</v>
-      </c>
-      <c r="N38" s="18">
-        <f t="shared" si="41"/>
-        <v>16.666666666664831</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39">
-        <v>6</v>
-      </c>
-      <c r="C39">
-        <v>29</v>
-      </c>
-      <c r="D39" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G39" s="6">
-        <v>45089</v>
-      </c>
-      <c r="H39" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I39" s="12">
-        <v>30</v>
-      </c>
-      <c r="J39">
-        <v>1.2201</v>
-      </c>
-      <c r="K39">
-        <v>1.2203999999999999</v>
-      </c>
-      <c r="M39" s="18">
-        <f t="shared" si="40"/>
-        <v>0.29999999999996696</v>
-      </c>
-      <c r="N39" s="18">
-        <f t="shared" si="41"/>
-        <v>9.9999999999988987</v>
-      </c>
-      <c r="O39" s="12">
-        <v>8.01</v>
-      </c>
-      <c r="P39" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="Q39" s="16">
-        <v>45091.125</v>
-      </c>
-      <c r="S39" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T39" s="12" t="b">
-        <f t="shared" ref="T39" si="52">IF(G39-F39&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U39" s="12" t="str">
-        <f t="shared" ref="U39" si="53">IF(AND(D39="Stock Solution", N39&gt;=90, N39&lt;=110), "Good", IF(AND(D39="DI", N39&gt;=-3.33, N39&lt;=3.33), "Good", IF(OR(D39&lt;&gt;"Stock Solution", D39&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40">
-        <v>9</v>
-      </c>
-      <c r="C40">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s">
-        <v>100</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G40" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H40" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I40" s="12">
-        <v>30</v>
-      </c>
-      <c r="J40">
-        <v>1.2010000000000001</v>
-      </c>
-      <c r="K40">
-        <v>1.2016</v>
-      </c>
-      <c r="M40" s="18">
-        <f t="shared" si="40"/>
-        <v>0.59999999999993392</v>
-      </c>
-      <c r="N40" s="18">
-        <f t="shared" si="41"/>
-        <v>19.999999999997797</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41">
-        <v>6</v>
-      </c>
-      <c r="C41">
-        <v>30</v>
-      </c>
-      <c r="D41" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G41" s="6">
-        <v>45089</v>
-      </c>
-      <c r="H41" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I41" s="12">
-        <v>30</v>
-      </c>
-      <c r="J41">
-        <v>1.2141999999999999</v>
-      </c>
-      <c r="K41">
-        <v>1.2141999999999999</v>
-      </c>
-      <c r="M41" s="18">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="N41" s="18">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="O41" s="12">
-        <v>7.97</v>
-      </c>
-      <c r="P41" s="12">
-        <v>0.21</v>
-      </c>
-      <c r="Q41" s="16">
-        <v>45091.125</v>
-      </c>
-      <c r="S41" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="T41" s="12" t="b">
-        <f t="shared" ref="T41" si="54">IF(G41-F41&gt;7, TRUE, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="U41" s="12" t="str">
-        <f t="shared" ref="U41" si="55">IF(AND(D41="Stock Solution", N41&gt;=90, N41&lt;=110), "Good", IF(AND(D41="DI", N41&gt;=-3.33, N41&lt;=3.33), "Good", IF(OR(D41&lt;&gt;"Stock Solution", D41&lt;&gt;"DI"), "", "Bad")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>95</v>
-      </c>
-      <c r="B42">
-        <v>9</v>
-      </c>
-      <c r="C42">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s">
-        <v>101</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="6">
-        <v>45085</v>
-      </c>
-      <c r="G42" s="6">
-        <v>45098</v>
-      </c>
-      <c r="H42" s="6">
-        <v>45102</v>
-      </c>
-      <c r="I42" s="12">
-        <v>30</v>
-      </c>
-      <c r="J42">
-        <v>1.2165999999999999</v>
-      </c>
-      <c r="K42">
-        <v>1.2170000000000001</v>
-      </c>
-      <c r="M42" s="18">
-        <f t="shared" si="40"/>
-        <v>0.40000000000017799</v>
-      </c>
-      <c r="N42" s="18">
-        <f t="shared" si="41"/>
-        <v>13.333333333339267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BD5783-6DE4-4462-AE79-C2E78620ED17}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.265625" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>55</v>
       </c>
@@ -5550,7 +3267,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -5589,7 +3306,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -5628,7 +3345,7 @@
         <v>-3.3333333333329662</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -5665,7 +3382,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -5703,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -5740,7 +3457,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -5777,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -5814,7 +3531,7 @@
         <v>100.00000000000379</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>3</v>
       </c>
@@ -5851,7 +3568,7 @@
         <v>-3.3333333333329662</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>6</v>
       </c>
@@ -5885,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -5919,7 +3636,7 @@
         <v>93.333333333337862</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -5954,7 +3671,7 @@
       </c>
       <c r="N12" s="18"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -5989,7 +3706,7 @@
       </c>
       <c r="N13" s="18"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>4</v>
       </c>
@@ -6026,7 +3743,7 @@
         <v>103.33333333332936</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>5</v>
       </c>
@@ -6063,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>4</v>
       </c>
@@ -6100,7 +3817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>4</v>
       </c>
@@ -6140,7 +3857,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -6180,7 +3897,7 @@
         <v>100.00000000000379</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -6220,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -6257,7 +3974,7 @@
         <v>96.666666666663431</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -6294,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -6331,7 +4048,7 @@
         <v>100.00000000000379</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -6368,7 +4085,7 @@
         <v>-3.3333333333329662</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -6405,7 +4122,7 @@
         <v>96.666666666670821</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -6442,7 +4159,7 @@
         <v>3.3333333333329662</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -6479,7 +4196,7 @@
         <v>106.66666666666973</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>11</v>
       </c>
@@ -6516,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12</v>
       </c>
@@ -6553,7 +4270,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -6590,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>13</v>
       </c>
@@ -6627,7 +4344,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>13</v>
       </c>
@@ -6664,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14</v>
       </c>
@@ -6701,7 +4418,7 @@
         <v>103.33333333333675</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>14</v>
       </c>
@@ -6738,7 +4455,7 @@
         <v>3.3333333333329662</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15</v>
       </c>
@@ -6775,7 +4492,7 @@
         <v>99.99999999999639</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15</v>
       </c>
@@ -6812,7 +4529,7 @@
         <v>3.3333333333329662</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>16</v>
       </c>
@@ -6849,7 +4566,7 @@
         <v>103.33333333333675</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16</v>
       </c>
@@ -6886,7 +4603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>17</v>
       </c>
@@ -6923,7 +4640,7 @@
         <v>103.33333333332936</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>17</v>
       </c>
@@ -6967,26 +4684,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678F2DA36292A241BB6B602A04ACAAD9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d9fb0f190deb5e7e937e6d8ad317d77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="167cb1e9-24b5-43e0-9f5d-14a54474cc90" xmlns:ns3="fbf6f0f6-9634-473c-8838-2f74fc79f714" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="211896cd03a7fb44aac70cae515804dc" ns2:_="" ns3:_="">
     <xsd:import namespace="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
@@ -7235,10 +4932,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="167cb1e9-24b5-43e0-9f5d-14a54474cc90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fbf6f0f6-9634-473c-8838-2f74fc79f714" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF83E157-1D15-4BA2-846C-E5B17F63B121}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFBBD27-ACF1-4801-B8AD-B8A884D06C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
+    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7255,20 +4983,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFBBD27-ACF1-4801-B8AD-B8A884D06C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF83E157-1D15-4BA2-846C-E5B17F63B121}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="167cb1e9-24b5-43e0-9f5d-14a54474cc90"/>
-    <ds:schemaRef ds:uri="fbf6f0f6-9634-473c-8838-2f74fc79f714"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>